<commit_message>
MVC - Core Sports Store App, 1
</commit_message>
<xml_diff>
--- a/Work Log.xlsx
+++ b/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\ISIT-322-Developing-Mobile-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A175118F-7C32-430B-A2B7-F954DB53A74C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC896C-5852-4936-8842-81AA00CD0EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24285" yWindow="-14010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>In Class Lab Exercise</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>MVC - Core Sports Store App, 1 - Chapter 8</t>
+  </si>
+  <si>
+    <t>MVC - Core Sports Store App, 1 - Chapter 9</t>
   </si>
 </sst>
 </file>
@@ -245,8 +248,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2884049A-816E-4C90-B00B-7E195DC02E6F}" name="Table1" displayName="Table1" ref="B2:F27" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="B2:F27" xr:uid="{5498F7FE-F847-48FF-BEDF-35E97F747022}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2884049A-816E-4C90-B00B-7E195DC02E6F}" name="Table1" displayName="Table1" ref="B2:F28" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B2:F28" xr:uid="{5498F7FE-F847-48FF-BEDF-35E97F747022}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{ABDEFB6A-23E8-490B-8BA3-31FDB8C966B2}" name="Assignment Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{E1FB43F5-1B65-45C1-AB26-4B96C8816E4F}" name="Time in hrs" dataDxfId="1"/>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F27"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,31 +797,46 @@
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>28</v>
+      <c r="B25" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2"/>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="1" t="s">
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
From book cp 10 & 11
</commit_message>
<xml_diff>
--- a/Work Log.xlsx
+++ b/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\ISIT-322-Developing-Mobile-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC896C-5852-4936-8842-81AA00CD0EC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C083F458-2269-4D0D-B8B8-7749ABEB7959}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24285" yWindow="-14010" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +769,9 @@
       <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>